<commit_message>
Added picklist for timezone and language fields, added integrer format to customisation import and export
</commit_message>
<xml_diff>
--- a/JosephM.CustomisationImporter.Test/TestCustomisations.xlsx
+++ b/JosephM.CustomisationImporter.Test/TestCustomisations.xlsx
@@ -1,20 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joseph.mcgregor-macd\Source\Repos\XRM-Developer-Tool\JosephM.CustomisationImporter.Test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13800" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Record Types" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="Fields" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="Option Sets" sheetId="3" r:id="rId5"/>
-    <sheet state="visible" name="Relationships" sheetId="4" r:id="rId6"/>
+    <sheet name="Record Types" sheetId="1" r:id="rId1"/>
+    <sheet name="Fields" sheetId="2" r:id="rId2"/>
+    <sheet name="Option Sets" sheetId="3" r:id="rId3"/>
+    <sheet name="Relationships" sheetId="4" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="126">
   <si>
     <t>Record Type Schema Name</t>
   </si>
@@ -359,23 +367,63 @@
   </si>
   <si>
     <t>A string field</t>
+  </si>
+  <si>
+    <t>new_duration</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>This is a duration</t>
+  </si>
+  <si>
+    <t>new_timezone</t>
+  </si>
+  <si>
+    <t>Timezone</t>
+  </si>
+  <si>
+    <t>This is a timezone</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>new_language</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>This is a language</t>
+  </si>
+  <si>
+    <t>Integer Format</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -383,61 +431,320 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4472C4"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="15.63"/>
-    <col customWidth="1" min="2" max="2" width="20.38"/>
-    <col customWidth="1" min="3" max="4" width="20.13"/>
-    <col customWidth="1" min="5" max="5" width="7.13"/>
-    <col customWidth="1" min="6" max="26" width="7.0"/>
+    <col min="1" max="1" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="26" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -487,7 +794,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" ht="16.5" customHeight="1">
+    <row r="2" spans="1:26" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -501,28 +808,28 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -536,57 +843,61 @@
         <v>24</v>
       </c>
       <c r="E3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="F3">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="S19" sqref="R17:S19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="22.13"/>
-    <col customWidth="1" min="2" max="2" width="15.13"/>
-    <col customWidth="1" min="3" max="3" width="18.38"/>
-    <col customWidth="1" min="4" max="4" width="13.63"/>
-    <col customWidth="1" min="5" max="6" width="21.0"/>
-    <col customWidth="1" min="7" max="7" width="11.5"/>
-    <col customWidth="1" min="8" max="8" width="7.13"/>
-    <col customWidth="1" min="9" max="11" width="10.75"/>
-    <col customWidth="1" min="12" max="13" width="13.75"/>
-    <col customWidth="1" min="14" max="14" width="12.75"/>
-    <col customWidth="1" min="15" max="16" width="10.75"/>
-    <col customWidth="1" min="17" max="17" width="11.63"/>
-    <col customWidth="1" min="18" max="19" width="11.5"/>
-    <col customWidth="1" min="20" max="20" width="39.38"/>
-    <col customWidth="1" min="21" max="26" width="7.0"/>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.140625" customWidth="1"/>
+    <col min="9" max="11" width="10.7109375" customWidth="1"/>
+    <col min="12" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="16" width="10.7109375" customWidth="1"/>
+    <col min="17" max="17" width="29.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" customWidth="1"/>
+    <col min="19" max="20" width="11.42578125" customWidth="1"/>
+    <col min="21" max="21" width="39.42578125" customWidth="1"/>
+    <col min="22" max="27" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,28 +944,31 @@
         <v>39</v>
       </c>
       <c r="P1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-    </row>
-    <row r="2">
+      <c r="AA1" s="1"/>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -683,39 +997,40 @@
         <v>1</v>
       </c>
       <c r="J2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="M2" t="b">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>200.0</v>
+        <v>200</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>50</v>
       </c>
       <c r="P2" s="1"/>
-      <c r="Q2" s="1">
-        <v>0.0</v>
-      </c>
+      <c r="Q2" s="1"/>
       <c r="R2" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="S2" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="T2" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="T2" s="1">
+        <v>4</v>
+      </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
       <c r="Z2" s="1"/>
-    </row>
-    <row r="3">
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -744,22 +1059,22 @@
         <v>0</v>
       </c>
       <c r="J3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="K3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="M3" t="b">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>200.0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>200</v>
+      </c>
+      <c r="T3" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -788,22 +1103,22 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K4">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="M4" t="b">
         <v>0</v>
       </c>
-      <c r="S4" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="T4" s="1">
+        <v>4</v>
+      </c>
+      <c r="U4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -832,22 +1147,22 @@
         <v>0</v>
       </c>
       <c r="J5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>125.0</v>
+        <v>125</v>
       </c>
       <c r="M5" t="b">
         <v>0</v>
       </c>
-      <c r="S5" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="T5" t="s">
+      <c r="T5" s="1">
+        <v>4</v>
+      </c>
+      <c r="U5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -876,25 +1191,25 @@
         <v>0</v>
       </c>
       <c r="J6">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="M6" t="b">
         <v>0</v>
       </c>
-      <c r="Q6">
-        <v>0.0</v>
-      </c>
       <c r="R6">
-        <v>100000.0</v>
-      </c>
-      <c r="S6" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>100000</v>
+      </c>
+      <c r="T6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -923,16 +1238,16 @@
         <v>0</v>
       </c>
       <c r="J7">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M7" t="b">
         <v>0</v>
       </c>
-      <c r="S7" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="T7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -963,14 +1278,14 @@
       <c r="M8" t="b">
         <v>0</v>
       </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
-      <c r="S8" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="Q8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1004,11 +1319,11 @@
       <c r="M9" t="b">
         <v>0</v>
       </c>
-      <c r="S9" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="T9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1037,22 +1352,22 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M10" t="b">
         <v>0</v>
       </c>
-      <c r="Q10">
-        <v>0.0</v>
-      </c>
       <c r="R10">
-        <v>100000.0</v>
-      </c>
-      <c r="S10" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>100000</v>
+      </c>
+      <c r="T10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1081,22 +1396,22 @@
         <v>0</v>
       </c>
       <c r="J11">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M11" t="b">
         <v>0</v>
       </c>
-      <c r="Q11">
-        <v>0.0</v>
-      </c>
       <c r="R11">
-        <v>100000.0</v>
-      </c>
-      <c r="S11" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="12">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>100000</v>
+      </c>
+      <c r="T11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1127,17 +1442,17 @@
       <c r="M12" t="b">
         <v>0</v>
       </c>
-      <c r="Q12">
-        <v>0.0</v>
-      </c>
       <c r="R12">
-        <v>100000.0</v>
-      </c>
-      <c r="S12" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>100000</v>
+      </c>
+      <c r="T12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1166,19 +1481,19 @@
         <v>0</v>
       </c>
       <c r="J13">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="M13" t="b">
         <v>0</v>
       </c>
       <c r="N13">
-        <v>100.0</v>
-      </c>
-      <c r="S13" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="14">
+        <v>100</v>
+      </c>
+      <c r="T13" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1207,22 +1522,22 @@
         <v>0</v>
       </c>
       <c r="J14">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M14" t="b">
         <v>0</v>
       </c>
       <c r="N14">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="O14" t="s">
         <v>98</v>
       </c>
-      <c r="S14" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="T14" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1251,22 +1566,22 @@
         <v>0</v>
       </c>
       <c r="J15">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M15" t="b">
         <v>0</v>
       </c>
       <c r="N15">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="O15" t="s">
         <v>100</v>
       </c>
-      <c r="S15" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="T15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1295,234 +1610,390 @@
         <v>0</v>
       </c>
       <c r="J16">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M16" t="b">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="O16" t="s">
         <v>105</v>
       </c>
-      <c r="S16" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="s">
+      <c r="T16" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="b">
+        <v>0</v>
+      </c>
+      <c r="G17" t="b">
+        <v>0</v>
+      </c>
+      <c r="H17" t="b">
+        <v>0</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <v>150</v>
+      </c>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>116</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <v>2147483647</v>
+      </c>
+      <c r="T17">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="b">
+        <v>0</v>
+      </c>
+      <c r="G18" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>3</v>
+      </c>
+      <c r="K18">
+        <v>150</v>
+      </c>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>121</v>
+      </c>
+      <c r="R18">
+        <v>-1500</v>
+      </c>
+      <c r="S18" s="3">
+        <v>1500</v>
+      </c>
+      <c r="T18">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D19" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" t="b">
+        <v>0</v>
+      </c>
+      <c r="G19" t="b">
+        <v>0</v>
+      </c>
+      <c r="H19" t="b">
+        <v>0</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>3</v>
+      </c>
+      <c r="K19">
+        <v>150</v>
+      </c>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>123</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>2147483647</v>
+      </c>
+      <c r="T19">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
         <v>106</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>107</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D20" t="s">
         <v>107</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E20" t="s">
         <v>108</v>
       </c>
-      <c r="F17" t="b">
-        <v>0</v>
-      </c>
-      <c r="G17" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17">
-        <v>1.0</v>
-      </c>
-      <c r="K17">
-        <v>100.0</v>
-      </c>
-      <c r="M17" t="b">
-        <v>0</v>
-      </c>
-      <c r="N17">
-        <v>2000.0</v>
-      </c>
-      <c r="S17" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="s">
+      <c r="F20" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>100</v>
+      </c>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>2000</v>
+      </c>
+      <c r="T20" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B21" t="s">
         <v>109</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>110</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D21" t="s">
         <v>111</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E21" t="s">
         <v>112</v>
       </c>
-      <c r="F18" t="b">
-        <v>0</v>
-      </c>
-      <c r="G18" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18">
-        <v>1.0</v>
-      </c>
-      <c r="K18">
-        <v>100.0</v>
-      </c>
-      <c r="M18" t="b">
-        <v>0</v>
-      </c>
-      <c r="N18">
-        <v>200.0</v>
-      </c>
-      <c r="S18" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="s">
+      <c r="F21" t="b">
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="K21">
+        <v>100</v>
+      </c>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>200</v>
+      </c>
+      <c r="T21" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C22" t="s">
         <v>113</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D22" t="s">
         <v>48</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E22" t="s">
         <v>114</v>
       </c>
-      <c r="F19" t="b">
-        <v>0</v>
-      </c>
-      <c r="G19" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19">
-        <v>1.0</v>
-      </c>
-      <c r="K19">
-        <v>100.0</v>
-      </c>
-      <c r="M19" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19">
-        <v>200.0</v>
-      </c>
-      <c r="S19" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="s">
+      <c r="F22" t="b">
+        <v>0</v>
+      </c>
+      <c r="G22" t="b">
+        <v>0</v>
+      </c>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <v>100</v>
+      </c>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>200</v>
+      </c>
+      <c r="T22" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B23" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C23" t="s">
         <v>47</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D23" t="s">
         <v>48</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E23" t="s">
         <v>49</v>
       </c>
-      <c r="F20" t="b">
-        <v>1</v>
-      </c>
-      <c r="G20" t="b">
-        <v>1</v>
-      </c>
-      <c r="H20" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20">
-        <v>1.0</v>
-      </c>
-      <c r="K20">
-        <v>200.0</v>
-      </c>
-      <c r="M20" t="b">
-        <v>0</v>
-      </c>
-      <c r="N20">
-        <v>200.0</v>
-      </c>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="1"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="T20" s="1"/>
+      <c r="F23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>200</v>
+      </c>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>200</v>
+      </c>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1">
+        <v>4</v>
+      </c>
+      <c r="U23" s="1"/>
     </row>
   </sheetData>
-  <dataValidations>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P19">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="Q22">
       <formula1>"Text,TextArea,Email,URL,TickerSymbol"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O1000">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P1"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="O2:O1003">
       <formula1>"Text,TextArea,Email,Url,TickerSymbol,Phone"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D1:D1000">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="D1:D1003">
       <formula1>"Boolean,Date,Decimal,Double,Integer,Lookup,Money,Picklist,String,Memo,Status"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt=" - " sqref="P2:P1048576">
+      <formula1>"None,Duration,TimeZone,Language,Locale"</formula1>
+    </dataValidation>
   </dataValidations>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="16.13"/>
-    <col customWidth="1" min="2" max="2" width="14.25"/>
-    <col customWidth="1" min="3" max="3" width="16.75"/>
-    <col customWidth="1" min="4" max="4" width="14.13"/>
-    <col customWidth="1" min="5" max="5" width="18.38"/>
-    <col customWidth="1" min="6" max="26" width="7.0"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="26" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1560,7 +2031,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -1568,13 +2039,13 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -1582,13 +2053,13 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1599,13 +2070,13 @@
         <v>1</v>
       </c>
       <c r="D4">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
@@ -1616,34 +2087,35 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="26.13"/>
-    <col customWidth="1" min="2" max="2" width="16.88"/>
-    <col customWidth="1" min="3" max="3" width="14.75"/>
-    <col customWidth="1" min="4" max="4" width="27.38"/>
-    <col customWidth="1" min="5" max="5" width="25.5"/>
-    <col customWidth="1" min="6" max="6" width="26.38"/>
-    <col customWidth="1" min="7" max="26" width="7.0"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.42578125" customWidth="1"/>
+    <col min="5" max="5" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" customWidth="1"/>
+    <col min="7" max="26" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -1678,7 +2150,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>88</v>
       </c>
@@ -1707,13 +2179,13 @@
         <v>89</v>
       </c>
       <c r="J2">
-        <v>15000.0</v>
+        <v>15000</v>
       </c>
       <c r="K2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -1745,10 +2217,10 @@
         <v>89</v>
       </c>
       <c r="K3">
-        <v>20000.0</v>
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>